<commit_message>
mis à jour classification des métiers propre
</commit_message>
<xml_diff>
--- a/data/histoire urbaine digitale classification metiers.xlsx
+++ b/data/histoire urbaine digitale classification metiers.xlsx
@@ -5,16 +5,17 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Julien/Documents/GitHub/HUM-450-Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Julien/Documents/GitHub/HUM-450-Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4F0B99-EE29-934E-9D87-8B0970154070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE3F489-4D80-8846-A5E8-8B08040E84D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{F8C1197D-2F23-A149-83C2-4E70C5CFBE33}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" activeTab="1" xr2:uid="{F8C1197D-2F23-A149-83C2-4E70C5CFBE33}"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="3" r:id="rId1"/>
-    <sheet name="infos" sheetId="4" r:id="rId2"/>
+    <sheet name="data_old" sheetId="3" r:id="rId1"/>
+    <sheet name="data" sheetId="5" r:id="rId2"/>
+    <sheet name="infos" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="190">
   <si>
     <t>rentiere</t>
   </si>
@@ -466,16 +467,164 @@
   </si>
   <si>
     <t>artisanat/service</t>
+  </si>
+  <si>
+    <t>rentier?</t>
+  </si>
+  <si>
+    <t>manœuvre</t>
+  </si>
+  <si>
+    <t>sans vocation</t>
+  </si>
+  <si>
+    <t>tailleur de pierres</t>
+  </si>
+  <si>
+    <t>gypseur/gypsier</t>
+  </si>
+  <si>
+    <t>marechal-ferrant</t>
+  </si>
+  <si>
+    <t>ecrivain</t>
+  </si>
+  <si>
+    <t>sage-femme</t>
+  </si>
+  <si>
+    <t>garde-malade</t>
+  </si>
+  <si>
+    <t>courtepointiere</t>
+  </si>
+  <si>
+    <t>juge d'appel</t>
+  </si>
+  <si>
+    <t>conseiller d'etat</t>
+  </si>
+  <si>
+    <t>teinturier</t>
+  </si>
+  <si>
+    <t>tailleur d'habits</t>
+  </si>
+  <si>
+    <t>secretaire</t>
+  </si>
+  <si>
+    <t>gendarme</t>
+  </si>
+  <si>
+    <t>notaire</t>
+  </si>
+  <si>
+    <t>loueur de chevaux</t>
+  </si>
+  <si>
+    <t>marchand de vin</t>
+  </si>
+  <si>
+    <t>procureur</t>
+  </si>
+  <si>
+    <t>tuilier</t>
+  </si>
+  <si>
+    <t>municipal</t>
+  </si>
+  <si>
+    <t>fournier</t>
+  </si>
+  <si>
+    <t>maitresse d'ecole</t>
+  </si>
+  <si>
+    <t>tourneur</t>
+  </si>
+  <si>
+    <t>coiffeur</t>
+  </si>
+  <si>
+    <t>conducteur de diligence</t>
+  </si>
+  <si>
+    <t>patissier</t>
+  </si>
+  <si>
+    <t>assistee</t>
+  </si>
+  <si>
+    <t>garde forestier</t>
+  </si>
+  <si>
+    <t>maitre valet</t>
+  </si>
+  <si>
+    <t>palefrenier</t>
+  </si>
+  <si>
+    <t>maitre de langue</t>
+  </si>
+  <si>
+    <t>gagne-denier</t>
+  </si>
+  <si>
+    <t>agent d'affaires</t>
+  </si>
+  <si>
+    <t>tapissier</t>
+  </si>
+  <si>
+    <t>vitrier</t>
+  </si>
+  <si>
+    <t>commis des peages</t>
+  </si>
+  <si>
+    <t>coutelier</t>
+  </si>
+  <si>
+    <t>marbrier</t>
+  </si>
+  <si>
+    <t>chaudronnier</t>
+  </si>
+  <si>
+    <t>assiste</t>
+  </si>
+  <si>
+    <t>mecanicien</t>
+  </si>
+  <si>
+    <t>revendeuse</t>
+  </si>
+  <si>
+    <t>ouvrier menuisier</t>
+  </si>
+  <si>
+    <t>artisanat/construction</t>
+  </si>
+  <si>
+    <t>administration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -501,7 +650,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -510,11 +659,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -848,8 +1040,8 @@
   <sheetPr codeName="Feuil3"/>
   <dimension ref="A1:B122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="G100" sqref="G100"/>
+    <sheetView topLeftCell="A84" zoomScale="141" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1836,10 +2028,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" stopIfTrue="1" operator="containsText" text="~?">
+    <cfRule type="containsText" dxfId="5" priority="1" stopIfTrue="1" operator="containsText" text="~?">
       <formula>NOT(ISERROR(SEARCH("~?",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" stopIfTrue="1" operator="containsText" text="/">
+    <cfRule type="containsText" dxfId="4" priority="2" stopIfTrue="1" operator="containsText" text="/">
       <formula>NOT(ISERROR(SEARCH("/",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1848,6 +2040,1056 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{880C3BB1-510F-BE43-A5CE-3DCBD22BD202}">
+  <dimension ref="A1:B127"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="191" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B47" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B50" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B51" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B52" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B53" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B54" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B55" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B56" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B57" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B58" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B59" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A61" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B61" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B62" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B63" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A65" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B65" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B66" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B67" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B68" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B69" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B70" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B71" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B72" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B73" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A74" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B74" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B75" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B76" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B77" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B78" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B79" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B80" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B81" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B82" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B83" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B84" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B85" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B86" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A87" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B87" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B88" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B89" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B90" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B91" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B92" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B93" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B94" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B95" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A96" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B96" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A97" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B97" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B98" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B99" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B100" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B101" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B102" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A103" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B103" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B104" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B105" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A106" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B106" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B107" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B108" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A109" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B109" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B110" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B111" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B112" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B113" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A114" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B114" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B115" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A116" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B116" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B117" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B118" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A119" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B119" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B120" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B121" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A122" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B122" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B123" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B124" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B125" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B126" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A127" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B127" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B1:B39 B41:B1048576">
+    <cfRule type="containsText" dxfId="3" priority="3" stopIfTrue="1" operator="containsText" text="~?">
+      <formula>NOT(ISERROR(SEARCH("~?",B1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" stopIfTrue="1" operator="containsText" text="/">
+      <formula>NOT(ISERROR(SEARCH("/",B1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40">
+    <cfRule type="containsText" dxfId="1" priority="1" stopIfTrue="1" operator="containsText" text="~?">
+      <formula>NOT(ISERROR(SEARCH("~?",B40)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" stopIfTrue="1" operator="containsText" text="/">
+      <formula>NOT(ISERROR(SEARCH("/",B40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D560CD-3C40-5143-95AE-8DA5116489EA}">
   <sheetPr codeName="Feuil4"/>
   <dimension ref="A1:C7"/>
@@ -1882,7 +3124,7 @@
         <v>101</v>
       </c>
       <c r="C2" s="3">
-        <f>COUNTIF(data!B:B,A2)</f>
+        <f>COUNTIF(data_old!B:B,A2)</f>
         <v>8</v>
       </c>
     </row>
@@ -1894,7 +3136,7 @@
         <v>102</v>
       </c>
       <c r="C3" s="3">
-        <f>COUNTIF(data!B:B,A3)</f>
+        <f>COUNTIF(data_old!B:B,A3)</f>
         <v>15</v>
       </c>
     </row>
@@ -1906,7 +3148,7 @@
         <v>46</v>
       </c>
       <c r="C4" s="3">
-        <f>COUNTIF(data!B:B,A4)</f>
+        <f>COUNTIF(data_old!B:B,A4)</f>
         <v>23</v>
       </c>
     </row>
@@ -1918,7 +3160,7 @@
         <v>47</v>
       </c>
       <c r="C5" s="3">
-        <f>COUNTIF(data!B:B,A5)</f>
+        <f>COUNTIF(data_old!B:B,A5)</f>
         <v>15</v>
       </c>
     </row>
@@ -1930,7 +3172,7 @@
         <v>45</v>
       </c>
       <c r="C6" s="3">
-        <f>COUNTIF(data!B:B,A6)</f>
+        <f>COUNTIF(data_old!B:B,A6)</f>
         <v>6</v>
       </c>
     </row>
@@ -1942,7 +3184,7 @@
         <v>103</v>
       </c>
       <c r="C7" s="3">
-        <f>COUNTIF(data!B:B,A7)</f>
+        <f>COUNTIF(data_old!B:B,A7)</f>
         <v>28</v>
       </c>
     </row>

</xml_diff>